<commit_message>
update menu KRITERIA 6
</commit_message>
<xml_diff>
--- a/Data-Kuantitatif-APS-Sarjana-Ver-1.0 (5).xlsx
+++ b/Data-Kuantitatif-APS-Sarjana-Ver-1.0 (5).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="8010" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="8835" firstSheet="30" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="MENU" sheetId="1" r:id="rId1"/>
@@ -3022,10 +3022,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -3105,6 +3105,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="24"/>
       <color rgb="FFFFC000"/>
@@ -3137,13 +3143,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -3297,12 +3296,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="1"/>
@@ -3319,7 +3318,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3526,43 +3525,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3869,19 +3838,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3974,41 +3943,41 @@
     <xf numFmtId="0" fontId="32" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4232,6 +4201,9 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4239,54 +4211,54 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="1"/>
@@ -4615,1069 +4587,1069 @@
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.89090909090909" style="84"/>
-    <col min="2" max="2" width="1.55454545454545" style="84" customWidth="1"/>
-    <col min="3" max="5" width="8.89090909090909" style="84"/>
-    <col min="6" max="6" width="10.6636363636364" style="84" customWidth="1"/>
-    <col min="7" max="7" width="3.55454545454545" style="84" customWidth="1"/>
-    <col min="8" max="8" width="8.89090909090909" style="84"/>
-    <col min="9" max="9" width="9.10909090909091" style="84" customWidth="1"/>
-    <col min="10" max="11" width="3.10909090909091" style="84" customWidth="1"/>
-    <col min="12" max="12" width="8.89090909090909" style="84"/>
-    <col min="13" max="13" width="4.10909090909091" style="84" customWidth="1"/>
-    <col min="14" max="14" width="2.44545454545455" style="84" customWidth="1"/>
-    <col min="15" max="16" width="8.89090909090909" style="84"/>
-    <col min="17" max="17" width="3.33636363636364" style="84" customWidth="1"/>
-    <col min="18" max="18" width="6.89090909090909" style="84" customWidth="1"/>
-    <col min="19" max="19" width="2.10909090909091" style="84" customWidth="1"/>
-    <col min="20" max="24" width="8.89090909090909" style="84"/>
-    <col min="25" max="25" width="1.66363636363636" style="84" customWidth="1"/>
-    <col min="26" max="16384" width="8.89090909090909" style="84"/>
+    <col min="1" max="1" width="8.8952380952381" style="85"/>
+    <col min="2" max="2" width="1.55238095238095" style="85" customWidth="1"/>
+    <col min="3" max="5" width="8.8952380952381" style="85"/>
+    <col min="6" max="6" width="10.6666666666667" style="85" customWidth="1"/>
+    <col min="7" max="7" width="3.55238095238095" style="85" customWidth="1"/>
+    <col min="8" max="8" width="8.8952380952381" style="85"/>
+    <col min="9" max="9" width="9.1047619047619" style="85" customWidth="1"/>
+    <col min="10" max="11" width="3.1047619047619" style="85" customWidth="1"/>
+    <col min="12" max="12" width="8.8952380952381" style="85"/>
+    <col min="13" max="13" width="4.1047619047619" style="85" customWidth="1"/>
+    <col min="14" max="14" width="2.44761904761905" style="85" customWidth="1"/>
+    <col min="15" max="16" width="8.8952380952381" style="85"/>
+    <col min="17" max="17" width="3.33333333333333" style="85" customWidth="1"/>
+    <col min="18" max="18" width="6.8952380952381" style="85" customWidth="1"/>
+    <col min="19" max="19" width="2.1047619047619" style="85" customWidth="1"/>
+    <col min="20" max="24" width="8.8952380952381" style="85"/>
+    <col min="25" max="25" width="1.66666666666667" style="85" customWidth="1"/>
+    <col min="26" max="16384" width="8.8952380952381" style="85"/>
   </cols>
   <sheetData>
     <row r="1" ht="1.95" customHeight="1" spans="1:25">
-      <c r="A1" s="85"/>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
+      <c r="A1" s="86"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
     </row>
     <row r="2" ht="30" spans="1:25">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
-    </row>
-    <row r="3" ht="23" spans="1:25">
-      <c r="A3" s="87" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
+      <c r="R2" s="87"/>
+      <c r="S2" s="87"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="87"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="87"/>
+      <c r="X2" s="87"/>
+      <c r="Y2" s="87"/>
+    </row>
+    <row r="3" ht="23.25" spans="1:25">
+      <c r="A3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+      <c r="T3" s="88"/>
+      <c r="U3" s="88"/>
+      <c r="V3" s="88"/>
+      <c r="W3" s="88"/>
+      <c r="X3" s="88"/>
+      <c r="Y3" s="88"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
     </row>
     <row r="5" ht="21" spans="1:25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="89" t="s">
+      <c r="A5" s="89"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="90" t="s">
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="97"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="97"/>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="97"/>
-      <c r="U5" s="97"/>
-      <c r="V5" s="97"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="88"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98"/>
+      <c r="T5" s="98"/>
+      <c r="U5" s="98"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
+      <c r="X5" s="105"/>
+      <c r="Y5" s="89"/>
     </row>
     <row r="6" ht="3" customHeight="1" spans="1:25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="88"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="88"/>
-      <c r="T6" s="88"/>
-      <c r="U6" s="88"/>
-      <c r="V6" s="88"/>
-      <c r="W6" s="88"/>
-      <c r="X6" s="88"/>
-      <c r="Y6" s="88"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
     </row>
     <row r="7" ht="21" spans="1:25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="89" t="s">
+      <c r="A7" s="89"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="90" t="s">
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
-      <c r="S7" s="88"/>
-      <c r="T7" s="88"/>
-      <c r="U7" s="88"/>
-      <c r="V7" s="88"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="88"/>
-      <c r="Y7" s="88"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="89"/>
+      <c r="S7" s="89"/>
+      <c r="T7" s="89"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="89"/>
+      <c r="W7" s="89"/>
+      <c r="X7" s="89"/>
+      <c r="Y7" s="89"/>
     </row>
     <row r="8" ht="3" customHeight="1" spans="1:25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="88"/>
-      <c r="L8" s="88"/>
-      <c r="M8" s="88"/>
-      <c r="N8" s="88"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="88"/>
-      <c r="Q8" s="88"/>
-      <c r="R8" s="88"/>
-      <c r="S8" s="88"/>
-      <c r="T8" s="88"/>
-      <c r="U8" s="88"/>
-      <c r="V8" s="88"/>
-      <c r="W8" s="88"/>
-      <c r="X8" s="88"/>
-      <c r="Y8" s="88"/>
+      <c r="A8" s="89"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
+      <c r="N8" s="89"/>
+      <c r="O8" s="89"/>
+      <c r="P8" s="89"/>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="89"/>
+      <c r="U8" s="89"/>
+      <c r="V8" s="89"/>
+      <c r="W8" s="89"/>
+      <c r="X8" s="89"/>
+      <c r="Y8" s="89"/>
     </row>
     <row r="9" ht="21" spans="1:25">
-      <c r="A9" s="88"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="89" t="s">
+      <c r="A9" s="89"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="93" t="s">
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="92"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-      <c r="L9" s="98"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="88"/>
-      <c r="R9" s="88"/>
-      <c r="S9" s="88"/>
-      <c r="T9" s="88"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="88"/>
-      <c r="W9" s="88"/>
-      <c r="X9" s="88"/>
-      <c r="Y9" s="88"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="89"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
     </row>
     <row r="10" ht="3" customHeight="1" spans="1:25">
-      <c r="A10" s="88"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="L10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="88"/>
-      <c r="X10" s="88"/>
-      <c r="Y10" s="88"/>
+      <c r="A10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
     </row>
     <row r="11" ht="21" spans="1:25">
-      <c r="A11" s="88"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89" t="s">
+      <c r="A11" s="89"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="93" t="s">
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="92"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="88"/>
-      <c r="S11" s="88"/>
-      <c r="T11" s="88"/>
-      <c r="U11" s="88"/>
-      <c r="V11" s="88"/>
-      <c r="W11" s="88"/>
-      <c r="X11" s="88"/>
-      <c r="Y11" s="88"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
     </row>
     <row r="12" ht="3" customHeight="1" spans="1:25">
-      <c r="A12" s="88"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88"/>
-      <c r="R12" s="88"/>
-      <c r="S12" s="88"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
-      <c r="W12" s="88"/>
-      <c r="X12" s="88"/>
-      <c r="Y12" s="88"/>
+      <c r="A12" s="89"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
     </row>
     <row r="13" ht="21" spans="1:25">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="89" t="s">
+      <c r="A13" s="89"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="93" t="s">
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="92"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="98"/>
-      <c r="Q13" s="98"/>
-      <c r="R13" s="98"/>
-      <c r="S13" s="98"/>
-      <c r="T13" s="98"/>
-      <c r="U13" s="98"/>
-      <c r="V13" s="98"/>
-      <c r="W13" s="98"/>
-      <c r="X13" s="99"/>
-      <c r="Y13" s="88"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="99"/>
+      <c r="P13" s="99"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="99"/>
+      <c r="S13" s="99"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="99"/>
+      <c r="V13" s="99"/>
+      <c r="W13" s="99"/>
+      <c r="X13" s="100"/>
+      <c r="Y13" s="89"/>
     </row>
     <row r="14" ht="3" customHeight="1" spans="1:25">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="88"/>
-      <c r="N14" s="88"/>
-      <c r="O14" s="88"/>
-      <c r="P14" s="88"/>
-      <c r="Q14" s="88"/>
-      <c r="R14" s="88"/>
-      <c r="S14" s="88"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="88"/>
-      <c r="V14" s="88"/>
-      <c r="W14" s="88"/>
-      <c r="X14" s="88"/>
-      <c r="Y14" s="88"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
     </row>
     <row r="15" ht="21" spans="1:25">
-      <c r="A15" s="88"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="89" t="s">
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="93" t="s">
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="92"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-      <c r="L15" s="98"/>
-      <c r="M15" s="98"/>
-      <c r="N15" s="98"/>
-      <c r="O15" s="98"/>
-      <c r="P15" s="98"/>
-      <c r="Q15" s="98"/>
-      <c r="R15" s="98"/>
-      <c r="S15" s="98"/>
-      <c r="T15" s="98"/>
-      <c r="U15" s="98"/>
-      <c r="V15" s="98"/>
-      <c r="W15" s="98"/>
-      <c r="X15" s="99"/>
-      <c r="Y15" s="88"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
+      <c r="P15" s="99"/>
+      <c r="Q15" s="99"/>
+      <c r="R15" s="99"/>
+      <c r="S15" s="99"/>
+      <c r="T15" s="99"/>
+      <c r="U15" s="99"/>
+      <c r="V15" s="99"/>
+      <c r="W15" s="99"/>
+      <c r="X15" s="100"/>
+      <c r="Y15" s="89"/>
     </row>
     <row r="16" ht="3" customHeight="1" spans="1:25">
-      <c r="A16" s="88"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
-      <c r="N16" s="88"/>
-      <c r="O16" s="88"/>
-      <c r="P16" s="88"/>
-      <c r="Q16" s="88"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="88"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="88"/>
-      <c r="V16" s="88"/>
-      <c r="W16" s="88"/>
-      <c r="X16" s="88"/>
-      <c r="Y16" s="88"/>
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="89"/>
+      <c r="M16" s="89"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="89"/>
+      <c r="P16" s="89"/>
+      <c r="Q16" s="89"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="89"/>
+      <c r="T16" s="89"/>
+      <c r="U16" s="89"/>
+      <c r="V16" s="89"/>
+      <c r="W16" s="89"/>
+      <c r="X16" s="89"/>
+      <c r="Y16" s="89"/>
     </row>
     <row r="17" ht="21" spans="1:25">
-      <c r="A17" s="88"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="89" t="s">
+      <c r="A17" s="89"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="88"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="92"/>
-      <c r="I17" s="98"/>
-      <c r="J17" s="98"/>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="98"/>
-      <c r="N17" s="98"/>
-      <c r="O17" s="98"/>
-      <c r="P17" s="98"/>
-      <c r="Q17" s="98"/>
-      <c r="R17" s="98"/>
-      <c r="S17" s="98"/>
-      <c r="T17" s="98"/>
-      <c r="U17" s="98"/>
-      <c r="V17" s="98"/>
-      <c r="W17" s="98"/>
-      <c r="X17" s="99"/>
-      <c r="Y17" s="88"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="99"/>
+      <c r="K17" s="99"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="99"/>
+      <c r="N17" s="99"/>
+      <c r="O17" s="99"/>
+      <c r="P17" s="99"/>
+      <c r="Q17" s="99"/>
+      <c r="R17" s="99"/>
+      <c r="S17" s="99"/>
+      <c r="T17" s="99"/>
+      <c r="U17" s="99"/>
+      <c r="V17" s="99"/>
+      <c r="W17" s="99"/>
+      <c r="X17" s="100"/>
+      <c r="Y17" s="89"/>
     </row>
     <row r="18" ht="3" customHeight="1" spans="1:25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="88"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="88"/>
-      <c r="J18" s="88"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="88"/>
-      <c r="M18" s="88"/>
-      <c r="N18" s="88"/>
-      <c r="O18" s="88"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="88"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="88"/>
-      <c r="T18" s="88"/>
-      <c r="U18" s="88"/>
-      <c r="V18" s="88"/>
-      <c r="W18" s="88"/>
-      <c r="X18" s="88"/>
-      <c r="Y18" s="88"/>
+      <c r="A18" s="89"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="89"/>
+      <c r="N18" s="89"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
+      <c r="Q18" s="89"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="89"/>
+      <c r="T18" s="89"/>
+      <c r="U18" s="89"/>
+      <c r="V18" s="89"/>
+      <c r="W18" s="89"/>
+      <c r="X18" s="89"/>
+      <c r="Y18" s="89"/>
     </row>
     <row r="19" ht="21" spans="1:25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="88"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="92"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="98"/>
-      <c r="P19" s="98"/>
-      <c r="Q19" s="98"/>
-      <c r="R19" s="98"/>
-      <c r="S19" s="98"/>
-      <c r="T19" s="98"/>
-      <c r="U19" s="98"/>
-      <c r="V19" s="98"/>
-      <c r="W19" s="98"/>
-      <c r="X19" s="99"/>
-      <c r="Y19" s="88"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="99"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="99"/>
+      <c r="P19" s="99"/>
+      <c r="Q19" s="99"/>
+      <c r="R19" s="99"/>
+      <c r="S19" s="99"/>
+      <c r="T19" s="99"/>
+      <c r="U19" s="99"/>
+      <c r="V19" s="99"/>
+      <c r="W19" s="99"/>
+      <c r="X19" s="100"/>
+      <c r="Y19" s="89"/>
     </row>
     <row r="20" ht="3" customHeight="1" spans="1:25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="88"/>
-      <c r="U20" s="88"/>
-      <c r="V20" s="88"/>
-      <c r="W20" s="88"/>
-      <c r="X20" s="88"/>
-      <c r="Y20" s="88"/>
+      <c r="A20" s="89"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="89"/>
+      <c r="N20" s="89"/>
+      <c r="O20" s="89"/>
+      <c r="P20" s="89"/>
+      <c r="Q20" s="89"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="89"/>
+      <c r="T20" s="89"/>
+      <c r="U20" s="89"/>
+      <c r="V20" s="89"/>
+      <c r="W20" s="89"/>
+      <c r="X20" s="89"/>
+      <c r="Y20" s="89"/>
     </row>
     <row r="21" ht="21" spans="1:25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="89" t="s">
+      <c r="A21" s="89"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="92"/>
-      <c r="M21" s="98"/>
-      <c r="N21" s="98"/>
-      <c r="O21" s="98"/>
-      <c r="P21" s="98"/>
-      <c r="Q21" s="98"/>
-      <c r="R21" s="98"/>
-      <c r="S21" s="98"/>
-      <c r="T21" s="99"/>
-      <c r="U21" s="89" t="s">
+      <c r="I21" s="89"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="101"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="99"/>
+      <c r="P21" s="99"/>
+      <c r="Q21" s="99"/>
+      <c r="R21" s="99"/>
+      <c r="S21" s="99"/>
+      <c r="T21" s="100"/>
+      <c r="U21" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="V21" s="100"/>
-      <c r="W21" s="105"/>
-      <c r="X21" s="105"/>
-      <c r="Y21" s="88"/>
+      <c r="V21" s="101"/>
+      <c r="W21" s="106"/>
+      <c r="X21" s="106"/>
+      <c r="Y21" s="89"/>
     </row>
     <row r="22" ht="3" customHeight="1" spans="1:25">
-      <c r="A22" s="88"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="88"/>
-      <c r="O22" s="88"/>
-      <c r="P22" s="88"/>
-      <c r="Q22" s="88"/>
-      <c r="R22" s="88"/>
-      <c r="S22" s="88"/>
-      <c r="T22" s="88"/>
-      <c r="U22" s="88"/>
-      <c r="V22" s="88"/>
-      <c r="W22" s="88"/>
-      <c r="X22" s="88"/>
-      <c r="Y22" s="88"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="89"/>
+      <c r="K22" s="89"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="89"/>
+      <c r="N22" s="89"/>
+      <c r="O22" s="89"/>
+      <c r="P22" s="89"/>
+      <c r="Q22" s="89"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="89"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="89"/>
+      <c r="V22" s="89"/>
+      <c r="W22" s="89"/>
+      <c r="X22" s="89"/>
+      <c r="Y22" s="89"/>
     </row>
     <row r="23" ht="21" spans="1:25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="89" t="s">
+      <c r="A23" s="89"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="93" t="s">
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="92"/>
-      <c r="I23" s="98"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="99"/>
-      <c r="M23" s="88"/>
-      <c r="N23" s="88"/>
-      <c r="O23" s="88"/>
-      <c r="P23" s="88"/>
-      <c r="Q23" s="88"/>
-      <c r="R23" s="88"/>
-      <c r="S23" s="88"/>
-      <c r="T23" s="88"/>
-      <c r="U23" s="88"/>
-      <c r="V23" s="88"/>
-      <c r="W23" s="88"/>
-      <c r="X23" s="88"/>
-      <c r="Y23" s="88"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="99"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="89"/>
+      <c r="O23" s="89"/>
+      <c r="P23" s="89"/>
+      <c r="Q23" s="89"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="89"/>
+      <c r="T23" s="89"/>
+      <c r="U23" s="89"/>
+      <c r="V23" s="89"/>
+      <c r="W23" s="89"/>
+      <c r="X23" s="89"/>
+      <c r="Y23" s="89"/>
     </row>
     <row r="24" ht="3" customHeight="1" spans="1:25">
-      <c r="A24" s="88"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="88"/>
-      <c r="L24" s="88"/>
-      <c r="M24" s="88"/>
-      <c r="N24" s="88"/>
-      <c r="O24" s="88"/>
-      <c r="P24" s="88"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="88"/>
-      <c r="S24" s="88"/>
-      <c r="T24" s="88"/>
-      <c r="U24" s="88"/>
-      <c r="V24" s="88"/>
-      <c r="W24" s="88"/>
-      <c r="X24" s="88"/>
-      <c r="Y24" s="88"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="89"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="89"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="89"/>
+      <c r="N24" s="89"/>
+      <c r="O24" s="89"/>
+      <c r="P24" s="89"/>
+      <c r="Q24" s="89"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="89"/>
+      <c r="U24" s="89"/>
+      <c r="V24" s="89"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="89"/>
+      <c r="Y24" s="89"/>
     </row>
     <row r="25" ht="21" spans="1:25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="89" t="s">
+      <c r="A25" s="89"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="88"/>
-      <c r="F25" s="88"/>
-      <c r="G25" s="93" t="s">
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="92"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-      <c r="O25" s="98"/>
-      <c r="P25" s="98"/>
-      <c r="Q25" s="98"/>
-      <c r="R25" s="99"/>
-      <c r="S25" s="88"/>
-      <c r="T25" s="88"/>
-      <c r="U25" s="88"/>
-      <c r="V25" s="88"/>
-      <c r="W25" s="88"/>
-      <c r="X25" s="88"/>
-      <c r="Y25" s="88"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="99"/>
+      <c r="J25" s="99"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="99"/>
+      <c r="N25" s="99"/>
+      <c r="O25" s="99"/>
+      <c r="P25" s="99"/>
+      <c r="Q25" s="99"/>
+      <c r="R25" s="100"/>
+      <c r="S25" s="89"/>
+      <c r="T25" s="89"/>
+      <c r="U25" s="89"/>
+      <c r="V25" s="89"/>
+      <c r="W25" s="89"/>
+      <c r="X25" s="89"/>
+      <c r="Y25" s="89"/>
     </row>
     <row r="26" ht="3" customHeight="1" spans="1:25">
-      <c r="A26" s="88"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="88"/>
-      <c r="T26" s="88"/>
-      <c r="U26" s="88"/>
-      <c r="V26" s="88"/>
-      <c r="W26" s="88"/>
-      <c r="X26" s="88"/>
-      <c r="Y26" s="88"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="89"/>
+      <c r="N26" s="89"/>
+      <c r="O26" s="89"/>
+      <c r="P26" s="89"/>
+      <c r="Q26" s="89"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="89"/>
+      <c r="T26" s="89"/>
+      <c r="U26" s="89"/>
+      <c r="V26" s="89"/>
+      <c r="W26" s="89"/>
+      <c r="X26" s="89"/>
+      <c r="Y26" s="89"/>
     </row>
     <row r="27" ht="21" spans="1:25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="89" t="s">
+      <c r="A27" s="89"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="93" t="s">
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="92"/>
-      <c r="I27" s="98"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="98"/>
-      <c r="L27" s="98"/>
-      <c r="M27" s="98"/>
-      <c r="N27" s="98"/>
-      <c r="O27" s="98"/>
-      <c r="P27" s="98"/>
-      <c r="Q27" s="98"/>
-      <c r="R27" s="99"/>
-      <c r="S27" s="88"/>
-      <c r="T27" s="88"/>
-      <c r="U27" s="88"/>
-      <c r="V27" s="88"/>
-      <c r="W27" s="88"/>
-      <c r="X27" s="88"/>
-      <c r="Y27" s="88"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
+      <c r="L27" s="99"/>
+      <c r="M27" s="99"/>
+      <c r="N27" s="99"/>
+      <c r="O27" s="99"/>
+      <c r="P27" s="99"/>
+      <c r="Q27" s="99"/>
+      <c r="R27" s="100"/>
+      <c r="S27" s="89"/>
+      <c r="T27" s="89"/>
+      <c r="U27" s="89"/>
+      <c r="V27" s="89"/>
+      <c r="W27" s="89"/>
+      <c r="X27" s="89"/>
+      <c r="Y27" s="89"/>
     </row>
     <row r="28" ht="3" customHeight="1" spans="1:25">
-      <c r="A28" s="88"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="88"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="88"/>
-      <c r="H28" s="88"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="88"/>
-      <c r="M28" s="88"/>
-      <c r="N28" s="88"/>
-      <c r="O28" s="88"/>
-      <c r="P28" s="88"/>
-      <c r="Q28" s="88"/>
-      <c r="R28" s="88"/>
-      <c r="S28" s="88"/>
-      <c r="T28" s="88"/>
-      <c r="U28" s="88"/>
-      <c r="V28" s="88"/>
-      <c r="W28" s="88"/>
-      <c r="X28" s="88"/>
-      <c r="Y28" s="88"/>
+      <c r="A28" s="89"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="89"/>
+      <c r="N28" s="89"/>
+      <c r="O28" s="89"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="89"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="89"/>
+      <c r="T28" s="89"/>
+      <c r="U28" s="89"/>
+      <c r="V28" s="89"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
+      <c r="Y28" s="89"/>
     </row>
     <row r="29" ht="21" spans="1:25">
-      <c r="A29" s="88"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="89" t="s">
+      <c r="A29" s="89"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="93" t="s">
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="94"/>
-      <c r="I29" s="101"/>
-      <c r="J29" s="93" t="s">
+      <c r="H29" s="95"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="94"/>
-      <c r="L29" s="102"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="88"/>
-      <c r="O29" s="88"/>
-      <c r="P29" s="88"/>
-      <c r="Q29" s="88"/>
-      <c r="R29" s="88"/>
-      <c r="S29" s="88"/>
-      <c r="T29" s="88"/>
-      <c r="U29" s="88"/>
-      <c r="V29" s="88"/>
-      <c r="W29" s="88"/>
-      <c r="X29" s="88"/>
-      <c r="Y29" s="88"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="103"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="89"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="89"/>
+      <c r="T29" s="89"/>
+      <c r="U29" s="89"/>
+      <c r="V29" s="89"/>
+      <c r="W29" s="89"/>
+      <c r="X29" s="89"/>
+      <c r="Y29" s="89"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="A30" s="88"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="88"/>
-      <c r="N30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="88"/>
-      <c r="R30" s="88"/>
-      <c r="S30" s="88"/>
-      <c r="T30" s="88"/>
-      <c r="U30" s="88"/>
-      <c r="V30" s="88"/>
-      <c r="W30" s="88"/>
-      <c r="X30" s="88"/>
-      <c r="Y30" s="88"/>
+      <c r="A30" s="89"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="L30" s="89"/>
+      <c r="M30" s="89"/>
+      <c r="N30" s="89"/>
+      <c r="O30" s="89"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="89"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
+      <c r="V30" s="89"/>
+      <c r="W30" s="89"/>
+      <c r="X30" s="89"/>
+      <c r="Y30" s="89"/>
     </row>
     <row r="31" ht="21" spans="1:25">
-      <c r="A31" s="88"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="95" t="s">
+      <c r="A31" s="89"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="88"/>
-      <c r="H31" s="88"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="89" t="s">
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="104"/>
+      <c r="O31" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="P31" s="88"/>
-      <c r="Q31" s="88"/>
-      <c r="R31" s="88"/>
-      <c r="S31" s="100" t="s">
+      <c r="P31" s="89"/>
+      <c r="Q31" s="89"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="T31" s="105"/>
-      <c r="U31" s="105"/>
-      <c r="V31" s="105"/>
-      <c r="W31" s="105"/>
-      <c r="X31" s="105"/>
-      <c r="Y31" s="88"/>
+      <c r="T31" s="106"/>
+      <c r="U31" s="106"/>
+      <c r="V31" s="106"/>
+      <c r="W31" s="106"/>
+      <c r="X31" s="106"/>
+      <c r="Y31" s="89"/>
     </row>
     <row r="32" ht="3" customHeight="1" spans="1:25">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
-      <c r="G32" s="88"/>
-      <c r="H32" s="88"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="88"/>
-      <c r="K32" s="88"/>
-      <c r="L32" s="88"/>
-      <c r="M32" s="88"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="88"/>
-      <c r="Q32" s="88"/>
-      <c r="R32" s="88"/>
-      <c r="S32" s="88"/>
-      <c r="T32" s="88"/>
-      <c r="U32" s="88"/>
-      <c r="V32" s="88"/>
-      <c r="W32" s="88"/>
-      <c r="X32" s="88"/>
-      <c r="Y32" s="88"/>
+      <c r="A32" s="89"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="104"/>
+      <c r="O32" s="101"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="89"/>
+      <c r="V32" s="89"/>
+      <c r="W32" s="89"/>
+      <c r="X32" s="89"/>
+      <c r="Y32" s="89"/>
     </row>
     <row r="33" ht="21" spans="1:25">
-      <c r="A33" s="88"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="88" t="s">
+      <c r="A33" s="89"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="88" t="s">
+      <c r="D33" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="106" t="s">
+      <c r="E33" s="107" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="88"/>
-      <c r="H33" s="88"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="88"/>
-      <c r="N33" s="103"/>
-      <c r="O33" s="89" t="s">
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="89"/>
+      <c r="K33" s="89"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="P33" s="88"/>
-      <c r="Q33" s="88"/>
-      <c r="R33" s="88"/>
-      <c r="S33" s="100" t="s">
+      <c r="P33" s="89"/>
+      <c r="Q33" s="89"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="T33" s="105"/>
-      <c r="U33" s="105"/>
-      <c r="V33" s="105"/>
-      <c r="W33" s="105"/>
-      <c r="X33" s="105"/>
-      <c r="Y33" s="88"/>
+      <c r="T33" s="106"/>
+      <c r="U33" s="106"/>
+      <c r="V33" s="106"/>
+      <c r="W33" s="106"/>
+      <c r="X33" s="106"/>
+      <c r="Y33" s="89"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="88"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
-      <c r="F34" s="88"/>
-      <c r="G34" s="88"/>
-      <c r="H34" s="88"/>
-      <c r="I34" s="88"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
-      <c r="O34" s="88"/>
-      <c r="P34" s="88"/>
-      <c r="Q34" s="88"/>
-      <c r="R34" s="88"/>
-      <c r="S34" s="88"/>
-      <c r="T34" s="88"/>
-      <c r="U34" s="88"/>
-      <c r="V34" s="88"/>
-      <c r="W34" s="88"/>
-      <c r="X34" s="88"/>
-      <c r="Y34" s="88"/>
+      <c r="A34" s="89"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="89"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="89"/>
+      <c r="N34" s="89"/>
+      <c r="O34" s="89"/>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="89"/>
+      <c r="S34" s="89"/>
+      <c r="T34" s="89"/>
+      <c r="U34" s="89"/>
+      <c r="V34" s="89"/>
+      <c r="W34" s="89"/>
+      <c r="X34" s="89"/>
+      <c r="Y34" s="89"/>
     </row>
     <row r="35" spans="1:25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="88"/>
-      <c r="N35" s="88"/>
-      <c r="O35" s="88"/>
-      <c r="P35" s="88"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
-      <c r="T35" s="88"/>
-      <c r="U35" s="88"/>
-      <c r="V35" s="88"/>
-      <c r="W35" s="88"/>
-      <c r="X35" s="88"/>
-      <c r="Y35" s="88"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="89"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="89"/>
+      <c r="O35" s="89"/>
+      <c r="P35" s="89"/>
+      <c r="Q35" s="89"/>
+      <c r="R35" s="89"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="89"/>
+      <c r="U35" s="89"/>
+      <c r="V35" s="89"/>
+      <c r="W35" s="89"/>
+      <c r="X35" s="89"/>
+      <c r="Y35" s="89"/>
     </row>
     <row r="36" ht="1.95" customHeight="1" spans="1:25">
-      <c r="A36" s="96"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="96"/>
-      <c r="D36" s="96"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="96"/>
-      <c r="J36" s="96"/>
-      <c r="K36" s="96"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="96"/>
-      <c r="N36" s="96"/>
-      <c r="O36" s="96"/>
-      <c r="P36" s="96"/>
-      <c r="Q36" s="96"/>
-      <c r="R36" s="96"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="96"/>
-      <c r="U36" s="96"/>
-      <c r="V36" s="96"/>
-      <c r="W36" s="96"/>
-      <c r="X36" s="96"/>
-      <c r="Y36" s="96"/>
+      <c r="A36" s="97"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="97"/>
+      <c r="S36" s="97"/>
+      <c r="T36" s="97"/>
+      <c r="U36" s="97"/>
+      <c r="V36" s="97"/>
+      <c r="W36" s="97"/>
+      <c r="X36" s="97"/>
+      <c r="Y36" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -5723,12 +5695,12 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.4454545454545" customWidth="1"/>
-    <col min="2" max="2" width="33.3363636363636" customWidth="1"/>
-    <col min="3" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="17.447619047619" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" customWidth="1"/>
+    <col min="3" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5872,12 +5844,12 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.4454545454545" customWidth="1"/>
-    <col min="2" max="2" width="33.3363636363636" customWidth="1"/>
-    <col min="3" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="17.447619047619" customWidth="1"/>
+    <col min="2" max="2" width="33.3333333333333" customWidth="1"/>
+    <col min="3" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6021,15 +5993,15 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="29.5545454545455" customWidth="1"/>
-    <col min="3" max="4" width="27.1090909090909" customWidth="1"/>
-    <col min="5" max="5" width="28.4454545454545" customWidth="1"/>
-    <col min="6" max="6" width="30.3363636363636" customWidth="1"/>
+    <col min="2" max="2" width="29.552380952381" customWidth="1"/>
+    <col min="3" max="4" width="27.1047619047619" customWidth="1"/>
+    <col min="5" max="5" width="28.447619047619" customWidth="1"/>
+    <col min="6" max="6" width="30.3333333333333" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="12.6636363636364" customWidth="1"/>
+    <col min="8" max="8" width="12.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6040,7 +6012,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" ht="29" spans="1:6">
+    <row r="4" ht="30" spans="1:6">
       <c r="A4" s="22" t="s">
         <v>149</v>
       </c>
@@ -6176,17 +6148,17 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="34.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="18.8909090909091" customWidth="1"/>
-    <col min="4" max="4" width="16.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="17.6636363636364" customWidth="1"/>
+    <col min="2" max="2" width="34.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="18.8952380952381" customWidth="1"/>
+    <col min="4" max="4" width="16.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="17.6666666666667" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="19.8909090909091" customWidth="1"/>
-    <col min="8" max="8" width="25.1090909090909" customWidth="1"/>
-    <col min="9" max="9" width="28.6636363636364" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="7" max="7" width="19.8952380952381" customWidth="1"/>
+    <col min="8" max="8" width="25.1047619047619" customWidth="1"/>
+    <col min="9" max="9" width="28.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -6473,16 +6445,16 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="39.8909090909091" customWidth="1"/>
-    <col min="3" max="3" width="14.6636363636364" customWidth="1"/>
-    <col min="4" max="5" width="16.3363636363636" customWidth="1"/>
-    <col min="6" max="6" width="18.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="19.1090909090909" customWidth="1"/>
-    <col min="8" max="8" width="23.5545454545455" customWidth="1"/>
-    <col min="9" max="9" width="26.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="39.8952380952381" customWidth="1"/>
+    <col min="3" max="3" width="14.6666666666667" customWidth="1"/>
+    <col min="4" max="5" width="16.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="18.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="19.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="23.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="26.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -6535,7 +6507,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="10" ht="29" spans="1:9">
+    <row r="10" ht="30" spans="1:9">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -6767,12 +6739,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="32.3363636363636" customWidth="1"/>
-    <col min="2" max="2" width="38.8909090909091" customWidth="1"/>
-    <col min="3" max="3" width="29.3363636363636" customWidth="1"/>
-    <col min="4" max="4" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="32.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="38.8952380952381" customWidth="1"/>
+    <col min="3" max="3" width="29.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6837,13 +6809,13 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.66363636363636" customWidth="1"/>
-    <col min="2" max="2" width="37.6636363636364" customWidth="1"/>
-    <col min="3" max="9" width="16.6636363636364" customWidth="1"/>
-    <col min="10" max="10" width="21.4454545454545" customWidth="1"/>
-    <col min="11" max="11" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="7.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="37.6666666666667" customWidth="1"/>
+    <col min="3" max="9" width="16.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="21.447619047619" customWidth="1"/>
+    <col min="11" max="11" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6880,7 +6852,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" ht="29" spans="1:10">
+    <row r="5" ht="30" spans="1:10">
       <c r="A5" s="13"/>
       <c r="B5" s="33"/>
       <c r="C5" s="22" t="s">
@@ -7153,15 +7125,15 @@
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.55454545454545" customWidth="1"/>
-    <col min="2" max="2" width="29.8909090909091" customWidth="1"/>
-    <col min="3" max="5" width="16.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="43.5545454545455" customWidth="1"/>
-    <col min="7" max="7" width="23.4454545454545" customWidth="1"/>
-    <col min="8" max="8" width="20.6636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="7.55238095238095" customWidth="1"/>
+    <col min="2" max="2" width="29.8952380952381" customWidth="1"/>
+    <col min="3" max="5" width="16.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="43.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="23.447619047619" customWidth="1"/>
+    <col min="8" max="8" width="20.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7384,15 +7356,15 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.55454545454545" customWidth="1"/>
-    <col min="2" max="2" width="29.8909090909091" customWidth="1"/>
-    <col min="3" max="5" width="16.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="43.5545454545455" customWidth="1"/>
-    <col min="7" max="7" width="25.7818181818182" customWidth="1"/>
-    <col min="8" max="8" width="22.8909090909091" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="7.55238095238095" customWidth="1"/>
+    <col min="2" max="2" width="29.8952380952381" customWidth="1"/>
+    <col min="3" max="5" width="16.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="43.552380952381" customWidth="1"/>
+    <col min="7" max="7" width="25.7809523809524" customWidth="1"/>
+    <col min="8" max="8" width="22.8952380952381" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -7408,7 +7380,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" ht="29" spans="1:8">
+    <row r="5" ht="30" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -7613,11 +7585,11 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="52.3363636363636" customWidth="1"/>
-    <col min="3" max="7" width="16.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="52.3333333333333" customWidth="1"/>
+    <col min="3" max="7" width="16.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7892,17 +7864,17 @@
   <sheetPr/>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="85.1090909090909" customWidth="1"/>
-    <col min="3" max="3" width="2.33636363636364" customWidth="1"/>
-    <col min="4" max="4" width="13.2181818181818" customWidth="1"/>
+    <col min="2" max="2" width="85.1047619047619" customWidth="1"/>
+    <col min="3" max="3" width="2.33333333333333" customWidth="1"/>
+    <col min="4" max="4" width="13.2190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" spans="1:4">
@@ -7993,7 +7965,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" ht="28" spans="1:4">
+    <row r="10" ht="28.5" spans="1:4">
       <c r="A10" s="75">
         <v>6</v>
       </c>
@@ -8041,7 +8013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" ht="28" spans="1:4">
+    <row r="14" ht="28.5" spans="1:4">
       <c r="A14" s="75">
         <v>10</v>
       </c>
@@ -8301,7 +8273,7 @@
         <v>89</v>
       </c>
       <c r="C35" s="77"/>
-      <c r="D35" s="79" t="s">
+      <c r="D35" s="83" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8317,7 +8289,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" ht="28.5" spans="1:4">
       <c r="A37" s="75">
         <v>33</v>
       </c>
@@ -8329,7 +8301,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" ht="28.5" spans="1:4">
       <c r="A38" s="75">
         <v>34</v>
       </c>
@@ -8517,7 +8489,7 @@
         <v>125</v>
       </c>
       <c r="C53" s="77"/>
-      <c r="D53" s="83" t="s">
+      <c r="D53" s="84" t="s">
         <v>126</v>
       </c>
     </row>
@@ -8596,13 +8568,13 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="33.3363636363636" customWidth="1"/>
-    <col min="4" max="4" width="16.4454545454545" customWidth="1"/>
-    <col min="5" max="7" width="12.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="21.7818181818182" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="3" width="33.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="16.447619047619" customWidth="1"/>
+    <col min="5" max="7" width="12.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="21.7809523809524" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -8845,7 +8817,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:D21">
       <formula1>$C$3:$C$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E21 F11:F21 G11:G21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:E21;F11:F21;G11:G21">
       <formula1>$B$4:$B$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -8869,15 +8841,15 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="37.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="23.6636363636364" customWidth="1"/>
-    <col min="4" max="4" width="22.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="20.4454545454545" customWidth="1"/>
-    <col min="6" max="6" width="18.2181818181818" customWidth="1"/>
+    <col min="2" max="2" width="37.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="23.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="22.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="20.447619047619" customWidth="1"/>
+    <col min="6" max="6" width="18.2190476190476" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9081,15 +9053,15 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="37.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="23.6636363636364" customWidth="1"/>
-    <col min="4" max="4" width="22.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="23.5545454545455" customWidth="1"/>
+    <col min="2" max="2" width="37.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="23.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="22.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="23.552380952381" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="26.1090909090909" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="7" max="7" width="26.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9293,15 +9265,15 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="37.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="23.6636363636364" customWidth="1"/>
-    <col min="4" max="4" width="22.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="23.5545454545455" customWidth="1"/>
+    <col min="2" max="2" width="37.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="23.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="22.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="23.552380952381" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="26.1090909090909" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="7" max="7" width="26.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9505,14 +9477,14 @@
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="44.3363636363636" customWidth="1"/>
-    <col min="3" max="3" width="22.6636363636364" customWidth="1"/>
-    <col min="4" max="4" width="21.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="22.3363636363636" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="44.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="22.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="21.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="22.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9558,7 +9530,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" ht="58" spans="1:6">
+    <row r="10" ht="60" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -9736,15 +9708,15 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="39.3363636363636" customWidth="1"/>
+    <col min="2" max="2" width="39.3333333333333" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="17.1090909090909" customWidth="1"/>
-    <col min="5" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="19.8909090909091" customWidth="1"/>
-    <col min="7" max="8" width="22.6636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="4" max="4" width="17.1047619047619" customWidth="1"/>
+    <col min="5" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="19.8952380952381" customWidth="1"/>
+    <col min="7" max="8" width="22.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -9780,7 +9752,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:8">
+    <row r="8" ht="30" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -9986,12 +9958,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="24.5545454545455" customWidth="1"/>
-    <col min="2" max="2" width="41.6636363636364" customWidth="1"/>
-    <col min="3" max="6" width="20.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="24.552380952381" customWidth="1"/>
+    <col min="2" max="2" width="41.6666666666667" customWidth="1"/>
+    <col min="3" max="6" width="20.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -10275,11 +10247,11 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="40.5545454545455" customWidth="1"/>
-    <col min="3" max="6" width="25.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="40.552380952381" customWidth="1"/>
+    <col min="3" max="6" width="25.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -10505,16 +10477,16 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="36.8952380952381" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.7818181818182" customWidth="1"/>
-    <col min="5" max="5" width="18.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
-    <col min="7" max="7" width="17.3363636363636" customWidth="1"/>
-    <col min="8" max="8" width="17.6636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="4" max="4" width="23.7809523809524" customWidth="1"/>
+    <col min="5" max="5" width="18.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
+    <col min="7" max="7" width="17.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="17.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -10802,16 +10774,16 @@
       <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="36.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="36.8952380952381" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="24.4454545454545" customWidth="1"/>
-    <col min="5" max="5" width="18.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
-    <col min="7" max="7" width="17.3363636363636" customWidth="1"/>
-    <col min="8" max="8" width="17.6636363636364" customWidth="1"/>
-    <col min="9" max="9" width="16.8909090909091" customWidth="1"/>
+    <col min="4" max="4" width="24.447619047619" customWidth="1"/>
+    <col min="5" max="5" width="18.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
+    <col min="7" max="7" width="17.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="17.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -11104,15 +11076,15 @@
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="19.3363636363636" customWidth="1"/>
-    <col min="4" max="8" width="16.6636363636364" customWidth="1"/>
-    <col min="9" max="9" width="12.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="12.4454545454545" customWidth="1"/>
-    <col min="11" max="11" width="15.8909090909091" customWidth="1"/>
-    <col min="12" max="12" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="13.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="19.3333333333333" customWidth="1"/>
+    <col min="4" max="8" width="16.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="12.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="12.447619047619" customWidth="1"/>
+    <col min="11" max="11" width="15.8952380952381" customWidth="1"/>
+    <col min="12" max="12" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11385,7 +11357,7 @@
     <mergeCell ref="K13:K14"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11 D16:D23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11;D16:D23">
       <formula1>$B$3:$B$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B23">
@@ -11413,14 +11385,14 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.3363636363636" customWidth="1"/>
-    <col min="3" max="4" width="15.6636363636364" customWidth="1"/>
-    <col min="5" max="7" width="11.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="12.6636363636364" customWidth="1"/>
+    <col min="2" max="2" width="37.3333333333333" customWidth="1"/>
+    <col min="3" max="4" width="15.6666666666667" customWidth="1"/>
+    <col min="5" max="7" width="11.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="12.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -11693,14 +11665,14 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.10909090909091" customWidth="1"/>
-    <col min="2" max="2" width="60.8909090909091" customWidth="1"/>
-    <col min="3" max="4" width="15.6636363636364" customWidth="1"/>
-    <col min="5" max="6" width="13.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="26.3363636363636" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="6.1047619047619" customWidth="1"/>
+    <col min="2" max="2" width="60.8952380952381" customWidth="1"/>
+    <col min="3" max="4" width="15.6666666666667" customWidth="1"/>
+    <col min="5" max="6" width="13.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="26.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -11961,17 +11933,17 @@
       <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.55454545454545" customWidth="1"/>
-    <col min="3" max="3" width="12.3363636363636" customWidth="1"/>
-    <col min="4" max="4" width="36.6636363636364" customWidth="1"/>
-    <col min="5" max="7" width="10.6636363636364" customWidth="1"/>
+    <col min="1" max="1" width="7.55238095238095" customWidth="1"/>
+    <col min="3" max="3" width="12.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="36.6666666666667" customWidth="1"/>
+    <col min="5" max="7" width="10.6666666666667" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="11" width="10.6636363636364" customWidth="1"/>
+    <col min="9" max="11" width="10.6666666666667" customWidth="1"/>
     <col min="12" max="12" width="22" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="16.8909090909091" customWidth="1"/>
+    <col min="14" max="14" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -12414,7 +12386,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B31">
       <formula1>$B$4:$B$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16:G31 I16:M31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16:G31;I16:M31">
       <formula1>$D$4:$D$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -12435,16 +12407,16 @@
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="36.5545454545455" customWidth="1"/>
-    <col min="3" max="3" width="59.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="31.1090909090909" customWidth="1"/>
-    <col min="5" max="5" width="29.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="36.552380952381" customWidth="1"/>
+    <col min="3" max="3" width="59.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="31.1047619047619" customWidth="1"/>
+    <col min="5" max="5" width="29.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12652,15 +12624,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="42.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="24.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="40.4454545454545" customWidth="1"/>
-    <col min="5" max="5" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="42.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="24.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="40.447619047619" customWidth="1"/>
+    <col min="5" max="5" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12772,15 +12744,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="26.6636363636364" customWidth="1"/>
-    <col min="4" max="4" width="40.8909090909091" customWidth="1"/>
-    <col min="5" max="5" width="16.8909090909091" customWidth="1"/>
+    <col min="3" max="3" width="26.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="40.8952380952381" customWidth="1"/>
+    <col min="5" max="5" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12791,7 +12763,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" ht="29" spans="1:4">
+    <row r="4" ht="30" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -12892,16 +12864,16 @@
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.1090909090909" customWidth="1"/>
-    <col min="3" max="10" width="12.6636363636364" customWidth="1"/>
-    <col min="11" max="11" width="24.2181818181818" customWidth="1"/>
-    <col min="12" max="12" width="19.3363636363636" customWidth="1"/>
-    <col min="13" max="13" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="37.1047619047619" customWidth="1"/>
+    <col min="3" max="10" width="12.6666666666667" customWidth="1"/>
+    <col min="11" max="11" width="24.2190476190476" customWidth="1"/>
+    <col min="12" max="12" width="19.3333333333333" customWidth="1"/>
+    <col min="13" max="13" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -13320,20 +13292,20 @@
   <sheetPr/>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="46.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="24.3363636363636" customWidth="1"/>
+    <col min="2" max="2" width="46.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="24.3333333333333" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="31.1090909090909" customWidth="1"/>
-    <col min="6" max="6" width="44.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="5" max="5" width="31.1047619047619" customWidth="1"/>
+    <col min="6" max="6" width="44.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -13535,15 +13507,15 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="37.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="27.3363636363636" customWidth="1"/>
-    <col min="4" max="4" width="21.1090909090909" customWidth="1"/>
+    <col min="2" max="2" width="37.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="27.3333333333333" customWidth="1"/>
+    <col min="4" max="4" width="21.1047619047619" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="21.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="25.3363636363636" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="6" max="6" width="21.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="25.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -13554,7 +13526,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" ht="29" spans="1:7">
+    <row r="4" ht="30" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -13740,12 +13712,12 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="42.3363636363636" customWidth="1"/>
-    <col min="3" max="5" width="20.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="44.3363636363636" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="42.3333333333333" customWidth="1"/>
+    <col min="3" max="5" width="20.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="44.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -13778,7 +13750,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="7" ht="29" spans="1:6">
+    <row r="7" ht="30" spans="1:6">
       <c r="A7" s="13"/>
       <c r="B7" s="33"/>
       <c r="C7" s="22" t="s">
@@ -13812,7 +13784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" ht="29" spans="1:6">
+    <row r="9" ht="30" spans="1:6">
       <c r="A9" s="20">
         <v>1</v>
       </c>
@@ -13824,7 +13796,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" ht="29" spans="1:6">
+    <row r="10" ht="30" spans="1:6">
       <c r="A10" s="20">
         <v>2</v>
       </c>
@@ -13836,7 +13808,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" ht="29" spans="1:6">
+    <row r="11" ht="30" spans="1:6">
       <c r="A11" s="20">
         <v>3</v>
       </c>
@@ -13848,7 +13820,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" ht="29" spans="1:6">
+    <row r="12" ht="30" spans="1:6">
       <c r="A12" s="20">
         <v>4</v>
       </c>
@@ -13860,7 +13832,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" ht="29" spans="1:6">
+    <row r="13" ht="30" spans="1:6">
       <c r="A13" s="20">
         <v>5</v>
       </c>
@@ -13872,7 +13844,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" ht="29" spans="1:6">
+    <row r="14" ht="30" spans="1:6">
       <c r="A14" s="20">
         <v>6</v>
       </c>
@@ -13892,7 +13864,7 @@
     <mergeCell ref="F6:F7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C14 D9:D14 E9:E14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C14;D9:D14;E9:E14">
       <formula1>$B$3:$B$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -13913,12 +13885,12 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="18.1090909090909" customWidth="1"/>
+    <col min="1" max="1" width="18.1047619047619" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="6" width="22.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="3" max="6" width="22.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14065,14 +14037,14 @@
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="15.3363636363636" customWidth="1"/>
-    <col min="3" max="3" width="47.1090909090909" customWidth="1"/>
-    <col min="4" max="4" width="25.8909090909091" customWidth="1"/>
-    <col min="5" max="5" width="19.3363636363636" customWidth="1"/>
-    <col min="6" max="7" width="32.3363636363636" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="15.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="47.1047619047619" customWidth="1"/>
+    <col min="4" max="4" width="25.8952380952381" customWidth="1"/>
+    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="6" max="7" width="32.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14103,7 +14075,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" ht="29" spans="1:7">
+    <row r="8" ht="30" spans="1:7">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -14351,15 +14323,15 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="15.3363636363636" customWidth="1"/>
-    <col min="3" max="3" width="47.1090909090909" customWidth="1"/>
-    <col min="4" max="4" width="25.8909090909091" customWidth="1"/>
-    <col min="5" max="5" width="19.3363636363636" customWidth="1"/>
-    <col min="6" max="6" width="31.1090909090909" customWidth="1"/>
-    <col min="7" max="7" width="30.1090909090909" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="15.3333333333333" customWidth="1"/>
+    <col min="3" max="3" width="47.1047619047619" customWidth="1"/>
+    <col min="4" max="4" width="25.8952380952381" customWidth="1"/>
+    <col min="5" max="5" width="19.3333333333333" customWidth="1"/>
+    <col min="6" max="6" width="31.1047619047619" customWidth="1"/>
+    <col min="7" max="7" width="30.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14385,7 +14357,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" ht="29" spans="1:7">
+    <row r="7" ht="30" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -14631,11 +14603,11 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="22.1090909090909" customWidth="1"/>
-    <col min="2" max="5" width="15.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="22.1047619047619" customWidth="1"/>
+    <col min="2" max="5" width="15.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14741,13 +14713,13 @@
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="31.4454545454545" customWidth="1"/>
-    <col min="3" max="3" width="49.1090909090909" customWidth="1"/>
-    <col min="4" max="4" width="16.8909090909091" customWidth="1"/>
-    <col min="5" max="7" width="12.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="31.447619047619" customWidth="1"/>
+    <col min="3" max="3" width="49.1047619047619" customWidth="1"/>
+    <col min="4" max="4" width="16.8952380952381" customWidth="1"/>
+    <col min="5" max="7" width="12.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14951,7 +14923,7 @@
     <mergeCell ref="D7:D8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E20 F10:F20 G10:G20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E20;F10:F20;G10:G20">
       <formula1>$B$3:$B$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -14973,13 +14945,13 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.3363636363636" customWidth="1"/>
-    <col min="2" max="2" width="17.3363636363636" customWidth="1"/>
-    <col min="3" max="9" width="12.6636363636364" customWidth="1"/>
-    <col min="10" max="10" width="17.6636363636364" customWidth="1"/>
-    <col min="11" max="12" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="16.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="17.3333333333333" customWidth="1"/>
+    <col min="3" max="9" width="12.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="17.6666666666667" customWidth="1"/>
+    <col min="11" max="12" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -15161,13 +15133,13 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.3363636363636" customWidth="1"/>
-    <col min="2" max="2" width="24.1090909090909" customWidth="1"/>
-    <col min="3" max="3" width="26.6636363636364" customWidth="1"/>
-    <col min="4" max="7" width="22.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="12.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="24.1047619047619" customWidth="1"/>
+    <col min="3" max="3" width="26.6666666666667" customWidth="1"/>
+    <col min="4" max="7" width="22.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -15290,13 +15262,13 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="12.3363636363636" customWidth="1"/>
-    <col min="2" max="2" width="23.8909090909091" customWidth="1"/>
-    <col min="3" max="3" width="25.4454545454545" customWidth="1"/>
-    <col min="4" max="6" width="22.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="12.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="23.8952380952381" customWidth="1"/>
+    <col min="3" max="3" width="25.447619047619" customWidth="1"/>
+    <col min="4" max="6" width="22.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -15411,13 +15383,13 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.44545454545455" customWidth="1"/>
+    <col min="1" max="1" width="6.44761904761905" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="6" width="16.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="40.8909090909091" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="3" max="6" width="16.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="40.8952380952381" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -15600,13 +15572,13 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="61.5545454545455" customWidth="1"/>
-    <col min="3" max="5" width="16.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="7.89090909090909" customWidth="1"/>
-    <col min="7" max="7" width="16.6636363636364" customWidth="1"/>
-    <col min="8" max="8" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="61.552380952381" customWidth="1"/>
+    <col min="3" max="5" width="16.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="7.8952380952381" customWidth="1"/>
+    <col min="7" max="7" width="16.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -15931,12 +15903,12 @@
       <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="35.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="69.1090909090909" customWidth="1"/>
-    <col min="4" max="4" width="16.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="35.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="69.1047619047619" customWidth="1"/>
+    <col min="4" max="4" width="16.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16083,18 +16055,18 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.66363636363636" customWidth="1"/>
-    <col min="2" max="2" width="43.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="12.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="12.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="13.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="41.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="22.4454545454545" customWidth="1"/>
-    <col min="8" max="8" width="11.5545454545455" customWidth="1"/>
-    <col min="9" max="9" width="20.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="43.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="13.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="41.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="22.447619047619" customWidth="1"/>
+    <col min="8" max="8" width="11.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="20.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16353,7 +16325,7 @@
     <mergeCell ref="I8:I9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C21 D11:D21 E11:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C21;D11:D21;E11:E21">
       <formula1>$B$4:$B$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -16376,13 +16348,13 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="44.5545454545455" customWidth="1"/>
-    <col min="3" max="3" width="30.5545454545455" customWidth="1"/>
-    <col min="4" max="4" width="45.6636363636364" customWidth="1"/>
-    <col min="5" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="44.552380952381" customWidth="1"/>
+    <col min="3" max="3" width="30.552380952381" customWidth="1"/>
+    <col min="4" max="4" width="45.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16546,12 +16518,12 @@
       <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="40.1090909090909" customWidth="1"/>
-    <col min="3" max="3" width="47.3363636363636" customWidth="1"/>
-    <col min="4" max="5" width="22.6636363636364" customWidth="1"/>
-    <col min="6" max="6" width="16.8909090909091" customWidth="1"/>
+    <col min="2" max="2" width="40.1047619047619" customWidth="1"/>
+    <col min="3" max="3" width="47.3333333333333" customWidth="1"/>
+    <col min="4" max="5" width="22.6666666666667" customWidth="1"/>
+    <col min="6" max="6" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16716,18 +16688,18 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.66363636363636" customWidth="1"/>
-    <col min="2" max="2" width="43.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="12.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="12.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="13.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="41.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="22.4454545454545" customWidth="1"/>
-    <col min="8" max="8" width="11.5545454545455" customWidth="1"/>
-    <col min="9" max="9" width="20.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="43.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="13.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="41.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="22.447619047619" customWidth="1"/>
+    <col min="8" max="8" width="11.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="20.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17009,18 +16981,18 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.66363636363636" customWidth="1"/>
-    <col min="2" max="2" width="43.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="12.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="12.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="13.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="41.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="22.4454545454545" customWidth="1"/>
-    <col min="8" max="8" width="11.5545454545455" customWidth="1"/>
-    <col min="9" max="9" width="20.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="43.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="13.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="41.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="22.447619047619" customWidth="1"/>
+    <col min="8" max="8" width="11.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="20.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17302,18 +17274,18 @@
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.66363636363636" customWidth="1"/>
-    <col min="2" max="2" width="43.6636363636364" customWidth="1"/>
-    <col min="3" max="3" width="12.4454545454545" customWidth="1"/>
-    <col min="4" max="4" width="12.3363636363636" customWidth="1"/>
-    <col min="5" max="5" width="13.5545454545455" customWidth="1"/>
-    <col min="6" max="6" width="41.6636363636364" customWidth="1"/>
-    <col min="7" max="7" width="22.4454545454545" customWidth="1"/>
-    <col min="8" max="8" width="11.5545454545455" customWidth="1"/>
-    <col min="9" max="9" width="20.8909090909091" customWidth="1"/>
-    <col min="10" max="10" width="16.8909090909091" customWidth="1"/>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="43.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.447619047619" customWidth="1"/>
+    <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="13.552380952381" customWidth="1"/>
+    <col min="6" max="6" width="41.6666666666667" customWidth="1"/>
+    <col min="7" max="7" width="22.447619047619" customWidth="1"/>
+    <col min="8" max="8" width="11.552380952381" customWidth="1"/>
+    <col min="9" max="9" width="20.8952380952381" customWidth="1"/>
+    <col min="10" max="10" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17595,15 +17567,15 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="14.6636363636364" customWidth="1"/>
-    <col min="2" max="2" width="20.1090909090909" customWidth="1"/>
-    <col min="3" max="3" width="18.3363636363636" customWidth="1"/>
+    <col min="1" max="1" width="14.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="20.1047619047619" customWidth="1"/>
+    <col min="3" max="3" width="18.3333333333333" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="19.8909090909091" customWidth="1"/>
-    <col min="7" max="7" width="16.8909090909091" customWidth="1"/>
+    <col min="6" max="6" width="19.8952380952381" customWidth="1"/>
+    <col min="7" max="7" width="16.8952380952381" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
upload bagian INDEX pada Kriteria 9 untuk semua sub
form masih on proses
</commit_message>
<xml_diff>
--- a/Data-Kuantitatif-APS-Sarjana-Ver-1.0 (5).xlsx
+++ b/Data-Kuantitatif-APS-Sarjana-Ver-1.0 (5).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8835" firstSheet="30" activeTab="36"/>
+    <workbookView windowWidth="20490" windowHeight="8835" firstSheet="36" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="MENU" sheetId="1" r:id="rId1"/>
@@ -3296,23 +3296,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="134"/>
@@ -7865,9 +7865,9 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -8381,7 +8381,7 @@
         <v>107</v>
       </c>
       <c r="C44" s="77"/>
-      <c r="D44" s="79" t="s">
+      <c r="D44" s="83" t="s">
         <v>108</v>
       </c>
     </row>
@@ -13292,10 +13292,10 @@
   <sheetPr/>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -14600,7 +14600,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -14710,7 +14710,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -14941,7 +14941,7 @@
   <sheetPr/>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>